<commit_message>
Testing .. 2 test case Fail
</commit_message>
<xml_diff>
--- a/Testing/Testing.xlsx
+++ b/Testing/Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Tase Case Name</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Case Description </t>
-  </si>
-  <si>
     <t>Test Case status Pass/Fail</t>
   </si>
   <si>
@@ -51,13 +48,73 @@
   </si>
   <si>
     <t>Aditya Parmar</t>
+  </si>
+  <si>
+    <t>Initial state</t>
+  </si>
+  <si>
+    <t>All the component render as expected</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Bonus Point Powerup</t>
+  </si>
+  <si>
+    <t>Add Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Speend </t>
+  </si>
+  <si>
+    <t>Add speed to Ball</t>
+  </si>
+  <si>
+    <t>Bullet Powerup</t>
+  </si>
+  <si>
+    <t>Kill all Object</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Not killing objects</t>
+  </si>
+  <si>
+    <t>Increse slider size power up</t>
+  </si>
+  <si>
+    <t>add width to slider</t>
+  </si>
+  <si>
+    <t>Decrese Slider Size Power up</t>
+  </si>
+  <si>
+    <t>Sub width to slider</t>
+  </si>
+  <si>
+    <t>Add extra ball Power Up</t>
+  </si>
+  <si>
+    <t>Add extra Ball</t>
+  </si>
+  <si>
+    <t>Game sholud stop all componet stop when game is over</t>
+  </si>
+  <si>
+    <t>Slider still move</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +135,13 @@
       <sz val="12"/>
       <color rgb="FF00B050"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -127,6 +191,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,13 +472,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
     <col min="3" max="3" width="54.1640625" customWidth="1"/>
     <col min="4" max="4" width="46.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
@@ -421,99 +487,195 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8">
+        <v>43088</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8">
+        <v>43089</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8">
+        <v>43090</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8">
+        <v>43091</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43092</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43093</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8">
+        <v>43094</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8">
+        <v>43095</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>